<commit_message>
docs: add a form to introduce the functions of each command
</commit_message>
<xml_diff>
--- a/ans/需要实现的指令集表.xlsx
+++ b/ans/需要实现的指令集表.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214F2967-FC39-4D18-B5F5-6CE212E3AB29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456F486D-D702-4EAF-9317-D36B1F2CCC1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="指令格式表" sheetId="1" r:id="rId1"/>
+    <sheet name="指令说明表" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="103">
   <si>
     <t>add</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -358,12 +359,126 @@
     <t>target [25:0]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>指令格式表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rd] = R[rs] + R[rt]</t>
+  </si>
+  <si>
+    <t>R[rd] = R[rs] - R[rt]</t>
+  </si>
+  <si>
+    <t>R[rd] = R[rs] &amp; R[rt]</t>
+  </si>
+  <si>
+    <t>R[rd] = R[rs] | R[rt]</t>
+  </si>
+  <si>
+    <t>R[rd] = R[rs] ^ R[rt]</t>
+  </si>
+  <si>
+    <t>R[rd] = ~(R[rs] | R[rt])</t>
+  </si>
+  <si>
+    <t>R[rd] = (R[rs]ø &lt; R[rt]ø) ? 1 : 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rd] = R[rt] &lt;&lt; shamt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rd] = (R[rs]± &lt; R[rt]±) ? 1 : 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rd] = R[rt]± &gt;&gt; shamt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rd] = R[rt]ø &gt;&gt; shamt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rt] = {imm, 16'b0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rt] = R[rs] + SignExtImm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rt] = R[rs] &amp; ZeroExtImm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rt] = (R[rs]ø &lt; SignExtImmø) ? 1 : 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[rt] = M[R[rs] + SignExtImm]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M[R[rs] + SignExtImm] = R[rt]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (R[rs] == R[rt]) PC += 4 + (offset &lt;&lt; 2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (R[rs] != R[rt]) PC += 4 + (offset &lt;&lt; 3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (R[rs] &lt;= 0) PC += 4 + (offset &lt;&lt; 4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (R[rs] &gt; 0) PC += 4 + (offset &lt;&lt; 5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (R[rs] &lt; 0) PC += 4 + (offset &lt;&lt; 6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC = {PC[31:28], target &lt;&lt; 2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[31] = PC + 4; PC = {PC[31:28], target &lt;&lt; 2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC = R[rs]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[31] = PC + 4; PC = R[rs]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指令说明表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,6 +506,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="黑体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -400,7 +529,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -423,16 +552,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -715,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -728,736 +919,1052 @@
     <col min="7" max="7" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="1">
         <v>3</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="1">
         <v>2</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F13" s="1">
         <v>3</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="2">
-        <v>0</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="2" t="s">
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="2">
-        <v>0</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2" t="s">
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="2">
-        <v>0</v>
-      </c>
-      <c r="G37" s="2" t="s">
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A24:G24"/>
+  <mergeCells count="24">
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
     <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="C35:G35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="D37:F37"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E29:G29"/>
     <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A19:G19"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D91AAE-118E-4614-9B05-D794CC443405}">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="48.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="8"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>